<commit_message>
CIERRE 20 SEP 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #08  AGOSTO  2023/INVENTARIO ALMACEN  AGOSTO  -2023 rtr.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #08  AGOSTO  2023/INVENTARIO ALMACEN  AGOSTO  -2023 rtr.xlsx
@@ -306,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="139">
   <si>
     <t>INVENTARIO ALMACEN</t>
   </si>
@@ -772,28 +772,34 @@
     <t>PECHUGA SH CONGELADA</t>
   </si>
   <si>
-    <t>ERROR DE BETY  REGISTRO UNA SALIDA DE CAMARON    100/200</t>
+    <t>ERROR DE BETY   INICIA EL MES  CON DIFERENTE PESOS Y CAJAS POR ESO ESTE RESULTADO</t>
   </si>
   <si>
-    <t>ERROR DE BETY  Registro salida 677-D1  con y cajas  y   SON 8 cajas   en Chambarete P</t>
+    <t xml:space="preserve">ERROR DE BETY  INICIA EL MES DE AGOSTSO    CON UNA CAJA MAS    4.54 kg  y 1 caja  </t>
   </si>
   <si>
-    <t xml:space="preserve">ERROR DE BETY  DIO SALIDAS DE MAS </t>
+    <t>ESTOS SON ERRORES DE   BETY DE ALMACEN</t>
+  </si>
+  <si>
+    <t>ESTOS SON LAS DIFERENCIAS CON EL INVENTARIO FISICO DE GERARDO</t>
+  </si>
+  <si>
+    <t>ERROR DE BETY  REGISTRO  SALIDA DE CAMARON    100/200---715-D1  La duplica con  el CAMARON  41/50</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ERROR DE BETY  INICIA CON UNA CAJA MAS   </t>
+      <t xml:space="preserve">ERROR DE BETY  Registro salida 677-D1  con 7  cajas  y   SON 8 cajas   en Chambarete P </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <sz val="16"/>
+        <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>NO SE DE DONDE ????</t>
+      <t xml:space="preserve"> ella registra 7 cajas</t>
     </r>
   </si>
 </sst>
@@ -806,7 +812,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="53" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1218,10 +1224,17 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="16"/>
       <name val="Calibri"/>
-      <family val="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1377,7 +1390,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="116">
+  <borders count="124">
     <border>
       <left/>
       <right/>
@@ -2844,13 +2857,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="568">
+  <cellXfs count="630">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4119,6 +4240,54 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4161,42 +4330,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="10" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4272,43 +4405,195 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="112" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="113" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="42" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="44" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="117" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="119" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="0" borderId="114" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="0" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="0" borderId="115" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="2" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="2" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="15" fillId="2" borderId="61" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="2" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="94" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="31" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="116" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="31" fillId="0" borderId="118" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="112" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="113" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="12" fillId="8" borderId="105" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="8" borderId="106" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="34" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="120" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="101" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="8" borderId="121" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="122" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="123" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="40" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
@@ -4319,11 +4604,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCCCFF"/>
       <color rgb="FF00CC00"/>
       <color rgb="FF00FFCC"/>
       <color rgb="FF800000"/>
       <color rgb="FFFFCCFF"/>
-      <color rgb="FFCCCCFF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FF9999FF"/>
       <color rgb="FFCCFF99"/>
@@ -4340,6 +4625,115 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>470647</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>22413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Cerrar llave 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9132794" y="3216089"/>
+          <a:ext cx="515471" cy="739588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>605118</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Cerrar llave 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11049000" y="3272117"/>
+          <a:ext cx="459442" cy="705971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4636,10 +5030,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="507"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -4651,21 +5045,21 @@
       <c r="P1" s="6"/>
     </row>
     <row r="2" spans="2:24" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="518">
+      <c r="B2" s="508">
         <v>44955</v>
       </c>
-      <c r="C2" s="519"/>
-      <c r="F2" s="520" t="s">
+      <c r="C2" s="509"/>
+      <c r="F2" s="510" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="520"/>
-      <c r="H2" s="520"/>
+      <c r="G2" s="510"/>
+      <c r="H2" s="510"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
-      <c r="K2" s="521" t="s">
+      <c r="K2" s="511" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="521"/>
+      <c r="L2" s="511"/>
       <c r="M2" s="9"/>
       <c r="N2" s="10"/>
       <c r="Q2" s="12"/>
@@ -4675,30 +5069,30 @@
     </row>
     <row r="3" spans="2:24" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="522" t="s">
+      <c r="C3" s="512" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="523"/>
+      <c r="D3" s="513"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="524" t="s">
+      <c r="F3" s="514" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="525"/>
+      <c r="G3" s="515"/>
       <c r="H3" s="15"/>
-      <c r="I3" s="526" t="s">
+      <c r="I3" s="516" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="16"/>
-      <c r="K3" s="521"/>
-      <c r="L3" s="521"/>
-      <c r="M3" s="503" t="s">
+      <c r="K3" s="511"/>
+      <c r="L3" s="511"/>
+      <c r="M3" s="519" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="504"/>
-      <c r="O3" s="505" t="s">
+      <c r="N3" s="520"/>
+      <c r="O3" s="521" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="506"/>
+      <c r="P3" s="522"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
@@ -4724,7 +5118,7 @@
       <c r="H4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="527"/>
+      <c r="I4" s="517"/>
       <c r="J4" s="16"/>
       <c r="K4" s="21" t="s">
         <v>10</v>
@@ -4785,8 +5179,8 @@
         <f>L5-I5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="507"/>
-      <c r="P5" s="507"/>
+      <c r="O5" s="523"/>
+      <c r="P5" s="523"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="13"/>
       <c r="S5" s="13"/>
@@ -4828,8 +5222,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O6" s="508"/>
-      <c r="P6" s="508"/>
+      <c r="O6" s="524"/>
+      <c r="P6" s="524"/>
       <c r="Q6" s="45"/>
       <c r="R6" s="13"/>
       <c r="S6" s="46"/>
@@ -4912,8 +5306,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O8" s="509"/>
-      <c r="P8" s="509"/>
+      <c r="O8" s="525"/>
+      <c r="P8" s="525"/>
       <c r="Q8" s="45"/>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
@@ -4994,8 +5388,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O10" s="510"/>
-      <c r="P10" s="510"/>
+      <c r="O10" s="526"/>
+      <c r="P10" s="526"/>
       <c r="Q10" s="45"/>
       <c r="R10" s="13"/>
       <c r="S10" s="13"/>
@@ -5123,8 +5517,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O13" s="511"/>
-      <c r="P13" s="511"/>
+      <c r="O13" s="527"/>
+      <c r="P13" s="527"/>
       <c r="Q13" s="45"/>
       <c r="R13" s="66"/>
       <c r="S13" s="66"/>
@@ -5392,8 +5786,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O20" s="512"/>
-      <c r="P20" s="512"/>
+      <c r="O20" s="528"/>
+      <c r="P20" s="528"/>
       <c r="Q20" s="45"/>
       <c r="R20" s="13"/>
       <c r="S20" s="13"/>
@@ -5478,8 +5872,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O22" s="513"/>
-      <c r="P22" s="513"/>
+      <c r="O22" s="529"/>
+      <c r="P22" s="529"/>
       <c r="Q22" s="45"/>
       <c r="R22" s="78"/>
       <c r="S22" s="78"/>
@@ -5521,8 +5915,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O23" s="514"/>
-      <c r="P23" s="514"/>
+      <c r="O23" s="530"/>
+      <c r="P23" s="530"/>
       <c r="Q23" s="45"/>
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
@@ -5644,8 +6038,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O26" s="515"/>
-      <c r="P26" s="515"/>
+      <c r="O26" s="531"/>
+      <c r="P26" s="531"/>
       <c r="Q26" s="45"/>
       <c r="R26" s="13"/>
       <c r="S26" s="13"/>
@@ -6158,10 +6552,10 @@
     <row r="40" spans="1:20" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="145"/>
       <c r="D40" s="147"/>
-      <c r="F40" s="502" t="s">
+      <c r="F40" s="518" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="502"/>
+      <c r="G40" s="518"/>
       <c r="H40" s="148">
         <f>SUM(H5:H31)</f>
         <v>51250.14</v>
@@ -6361,13 +6755,6 @@
     <sortCondition ref="B5:B38"/>
   </sortState>
   <mergeCells count="19">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
@@ -6380,6 +6767,13 @@
     <mergeCell ref="O22:P22"/>
     <mergeCell ref="O23:P23"/>
     <mergeCell ref="O26:P26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.15748031496062992" top="0.31496062992125984" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="78" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6446,10 +6840,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="507"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -6464,26 +6858,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="528">
+      <c r="B2" s="532">
         <v>44989</v>
       </c>
-      <c r="C2" s="529"/>
-      <c r="F2" s="530" t="s">
+      <c r="C2" s="533"/>
+      <c r="F2" s="534" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="531"/>
-      <c r="H2" s="532"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="534" t="s">
+      <c r="G2" s="535"/>
+      <c r="H2" s="536"/>
+      <c r="I2" s="537"/>
+      <c r="J2" s="538" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="534"/>
-      <c r="L2" s="535"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="539"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="521" t="s">
+      <c r="N2" s="511" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="521"/>
+      <c r="O2" s="511"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -6493,33 +6887,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="538" t="s">
+      <c r="C3" s="542" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="539"/>
+      <c r="D3" s="543"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="540" t="s">
+      <c r="F3" s="544" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="541"/>
+      <c r="G3" s="545"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="542" t="s">
+      <c r="I3" s="546" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="536"/>
-      <c r="K3" s="536"/>
-      <c r="L3" s="537"/>
+      <c r="J3" s="540"/>
+      <c r="K3" s="540"/>
+      <c r="L3" s="541"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="521"/>
-      <c r="O3" s="521"/>
-      <c r="P3" s="503" t="s">
+      <c r="N3" s="511"/>
+      <c r="O3" s="511"/>
+      <c r="P3" s="519" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="504"/>
-      <c r="R3" s="505" t="s">
+      <c r="Q3" s="520"/>
+      <c r="R3" s="521" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="506"/>
+      <c r="S3" s="522"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -6545,7 +6939,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="543"/>
+      <c r="I4" s="547"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -6621,8 +7015,8 @@
       <c r="Q5" s="38">
         <v>0</v>
       </c>
-      <c r="R5" s="507"/>
-      <c r="S5" s="507"/>
+      <c r="R5" s="523"/>
+      <c r="S5" s="523"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -6659,8 +7053,8 @@
         <f>O6-I6</f>
         <v>0</v>
       </c>
-      <c r="R6" s="508"/>
-      <c r="S6" s="508"/>
+      <c r="R6" s="524"/>
+      <c r="S6" s="524"/>
       <c r="T6" s="45"/>
       <c r="U6" s="13"/>
       <c r="V6" s="46"/>
@@ -6747,8 +7141,8 @@
       <c r="Q8" s="52">
         <v>0</v>
       </c>
-      <c r="R8" s="509"/>
-      <c r="S8" s="509"/>
+      <c r="R8" s="525"/>
+      <c r="S8" s="525"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -6835,8 +7229,8 @@
       <c r="Q10" s="52">
         <v>0</v>
       </c>
-      <c r="R10" s="510"/>
-      <c r="S10" s="510"/>
+      <c r="R10" s="526"/>
+      <c r="S10" s="526"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -6976,8 +7370,8 @@
       <c r="Q13" s="52">
         <v>0</v>
       </c>
-      <c r="R13" s="511"/>
-      <c r="S13" s="511"/>
+      <c r="R13" s="527"/>
+      <c r="S13" s="527"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -7285,8 +7679,8 @@
       <c r="Q20" s="52">
         <v>0</v>
       </c>
-      <c r="R20" s="512"/>
-      <c r="S20" s="512"/>
+      <c r="R20" s="528"/>
+      <c r="S20" s="528"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -7373,8 +7767,8 @@
       <c r="Q22" s="52">
         <v>0</v>
       </c>
-      <c r="R22" s="513"/>
-      <c r="S22" s="513"/>
+      <c r="R22" s="529"/>
+      <c r="S22" s="529"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -7420,8 +7814,8 @@
       <c r="Q23" s="52">
         <v>0</v>
       </c>
-      <c r="R23" s="514"/>
-      <c r="S23" s="514"/>
+      <c r="R23" s="530"/>
+      <c r="S23" s="530"/>
       <c r="T23" s="45"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
@@ -7561,8 +7955,8 @@
       <c r="Q26" s="52">
         <v>0</v>
       </c>
-      <c r="R26" s="515"/>
-      <c r="S26" s="515"/>
+      <c r="R26" s="531"/>
+      <c r="S26" s="531"/>
       <c r="T26" s="45"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
@@ -8245,10 +8639,10 @@
     <row r="43" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="145"/>
       <c r="D43" s="147"/>
-      <c r="F43" s="502" t="s">
+      <c r="F43" s="518" t="s">
         <v>46</v>
       </c>
-      <c r="G43" s="502"/>
+      <c r="G43" s="518"/>
       <c r="H43" s="148">
         <f>SUM(H5:H34)</f>
         <v>52842.86</v>
@@ -8469,14 +8863,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -8489,6 +8875,14 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.35" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8531,10 +8925,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="507"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -8549,26 +8943,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="528">
+      <c r="B2" s="532">
         <v>45017</v>
       </c>
-      <c r="C2" s="529"/>
-      <c r="F2" s="530" t="s">
+      <c r="C2" s="533"/>
+      <c r="F2" s="534" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="531"/>
-      <c r="H2" s="532"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="534" t="s">
+      <c r="G2" s="535"/>
+      <c r="H2" s="536"/>
+      <c r="I2" s="537"/>
+      <c r="J2" s="538" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="534"/>
-      <c r="L2" s="535"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="539"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="521" t="s">
+      <c r="N2" s="511" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="521"/>
+      <c r="O2" s="511"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -8578,33 +8972,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="538" t="s">
+      <c r="C3" s="542" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="539"/>
+      <c r="D3" s="543"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="540" t="s">
+      <c r="F3" s="544" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="541"/>
+      <c r="G3" s="545"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="542" t="s">
+      <c r="I3" s="546" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="536"/>
-      <c r="K3" s="536"/>
-      <c r="L3" s="537"/>
+      <c r="J3" s="540"/>
+      <c r="K3" s="540"/>
+      <c r="L3" s="541"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="521"/>
-      <c r="O3" s="521"/>
-      <c r="P3" s="503" t="s">
+      <c r="N3" s="511"/>
+      <c r="O3" s="511"/>
+      <c r="P3" s="519" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="504"/>
-      <c r="R3" s="505" t="s">
+      <c r="Q3" s="520"/>
+      <c r="R3" s="521" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="506"/>
+      <c r="S3" s="522"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -8630,7 +9024,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="543"/>
+      <c r="I4" s="547"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -8705,8 +9099,8 @@
         <f>O5-I5</f>
         <v>0</v>
       </c>
-      <c r="R5" s="507"/>
-      <c r="S5" s="507"/>
+      <c r="R5" s="523"/>
+      <c r="S5" s="523"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -8759,8 +9153,8 @@
         <f>O6-I6</f>
         <v>-2</v>
       </c>
-      <c r="R6" s="508"/>
-      <c r="S6" s="508"/>
+      <c r="R6" s="524"/>
+      <c r="S6" s="524"/>
       <c r="T6" s="180" t="s">
         <v>79</v>
       </c>
@@ -8865,8 +9259,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R8" s="509"/>
-      <c r="S8" s="509"/>
+      <c r="R8" s="525"/>
+      <c r="S8" s="525"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -8953,8 +9347,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R10" s="510"/>
-      <c r="S10" s="510"/>
+      <c r="R10" s="526"/>
+      <c r="S10" s="526"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -9105,8 +9499,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R13" s="511"/>
-      <c r="S13" s="511"/>
+      <c r="R13" s="527"/>
+      <c r="S13" s="527"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -9439,8 +9833,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R20" s="512"/>
-      <c r="S20" s="512"/>
+      <c r="R20" s="528"/>
+      <c r="S20" s="528"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -9527,8 +9921,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R22" s="513"/>
-      <c r="S22" s="513"/>
+      <c r="R22" s="529"/>
+      <c r="S22" s="529"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -9577,8 +9971,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R23" s="514"/>
-      <c r="S23" s="514"/>
+      <c r="R23" s="530"/>
+      <c r="S23" s="530"/>
       <c r="T23" s="180" t="s">
         <v>80</v>
       </c>
@@ -9717,8 +10111,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R26" s="515"/>
-      <c r="S26" s="515"/>
+      <c r="R26" s="531"/>
+      <c r="S26" s="531"/>
       <c r="T26" s="45"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
@@ -10822,10 +11216,10 @@
     <row r="51" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="544" t="s">
+      <c r="F51" s="548" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="544"/>
+      <c r="G51" s="548"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>74525.02</v>
@@ -11053,14 +11447,6 @@
     <sortCondition ref="B5:B50"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -11073,6 +11459,14 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.31" bottom="0.3" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="90" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11115,10 +11509,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="507"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -11133,26 +11527,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="528">
+      <c r="B2" s="532">
         <v>45056</v>
       </c>
-      <c r="C2" s="529"/>
-      <c r="F2" s="530" t="s">
+      <c r="C2" s="533"/>
+      <c r="F2" s="534" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="531"/>
-      <c r="H2" s="532"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="534" t="s">
+      <c r="G2" s="535"/>
+      <c r="H2" s="536"/>
+      <c r="I2" s="537"/>
+      <c r="J2" s="538" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="534"/>
-      <c r="L2" s="535"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="539"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="521" t="s">
+      <c r="N2" s="511" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="521"/>
+      <c r="O2" s="511"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -11162,33 +11556,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="538" t="s">
+      <c r="C3" s="542" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="539"/>
+      <c r="D3" s="543"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="540" t="s">
+      <c r="F3" s="544" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="541"/>
+      <c r="G3" s="545"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="542" t="s">
+      <c r="I3" s="546" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="536"/>
-      <c r="K3" s="536"/>
-      <c r="L3" s="537"/>
+      <c r="J3" s="540"/>
+      <c r="K3" s="540"/>
+      <c r="L3" s="541"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="521"/>
-      <c r="O3" s="521"/>
-      <c r="P3" s="503" t="s">
+      <c r="N3" s="511"/>
+      <c r="O3" s="511"/>
+      <c r="P3" s="519" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="504"/>
-      <c r="R3" s="505" t="s">
+      <c r="Q3" s="520"/>
+      <c r="R3" s="521" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="506"/>
+      <c r="S3" s="522"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -11214,7 +11608,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="543"/>
+      <c r="I4" s="547"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -11285,8 +11679,8 @@
         <f>I5-L5</f>
         <v>0</v>
       </c>
-      <c r="R5" s="507"/>
-      <c r="S5" s="507"/>
+      <c r="R5" s="523"/>
+      <c r="S5" s="523"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -11335,8 +11729,8 @@
         <f>I6-L6</f>
         <v>0</v>
       </c>
-      <c r="R6" s="508"/>
-      <c r="S6" s="508"/>
+      <c r="R6" s="524"/>
+      <c r="S6" s="524"/>
       <c r="T6" s="180"/>
       <c r="U6" s="13"/>
       <c r="V6" s="46"/>
@@ -11431,8 +11825,8 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="R8" s="509"/>
-      <c r="S8" s="509"/>
+      <c r="R8" s="525"/>
+      <c r="S8" s="525"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -11507,8 +11901,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R10" s="510"/>
-      <c r="S10" s="510"/>
+      <c r="R10" s="526"/>
+      <c r="S10" s="526"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -11629,8 +12023,8 @@
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
-      <c r="R13" s="511"/>
-      <c r="S13" s="511"/>
+      <c r="R13" s="527"/>
+      <c r="S13" s="527"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -11911,8 +12305,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R20" s="512"/>
-      <c r="S20" s="512"/>
+      <c r="R20" s="528"/>
+      <c r="S20" s="528"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -11987,8 +12381,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R22" s="513"/>
-      <c r="S22" s="513"/>
+      <c r="R22" s="529"/>
+      <c r="S22" s="529"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -12033,8 +12427,8 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
-      <c r="R23" s="514"/>
-      <c r="S23" s="514"/>
+      <c r="R23" s="530"/>
+      <c r="S23" s="530"/>
       <c r="T23" s="180"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
@@ -12163,8 +12557,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R26" s="515"/>
-      <c r="S26" s="515"/>
+      <c r="R26" s="531"/>
+      <c r="S26" s="531"/>
       <c r="T26" s="45"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
@@ -13170,10 +13564,10 @@
     <row r="51" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="544" t="s">
+      <c r="F51" s="548" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="544"/>
+      <c r="G51" s="548"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>51160.97</v>
@@ -13396,6 +13790,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -13408,14 +13810,6 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31496062992125984" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -13459,10 +13853,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="507"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -13477,26 +13871,26 @@
       <c r="S1" s="6"/>
     </row>
     <row r="2" spans="2:27" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="528">
+      <c r="B2" s="532">
         <v>45082</v>
       </c>
-      <c r="C2" s="529"/>
-      <c r="F2" s="530" t="s">
+      <c r="C2" s="533"/>
+      <c r="F2" s="534" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="531"/>
-      <c r="H2" s="532"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="534" t="s">
+      <c r="G2" s="535"/>
+      <c r="H2" s="536"/>
+      <c r="I2" s="537"/>
+      <c r="J2" s="538" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="534"/>
-      <c r="L2" s="535"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="539"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="521" t="s">
+      <c r="N2" s="511" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="521"/>
+      <c r="O2" s="511"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="10"/>
       <c r="T2" s="12"/>
@@ -13506,33 +13900,33 @@
     </row>
     <row r="3" spans="2:27" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="538" t="s">
+      <c r="C3" s="542" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="539"/>
+      <c r="D3" s="543"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="540" t="s">
+      <c r="F3" s="544" t="s">
         <v>93</v>
       </c>
-      <c r="G3" s="541"/>
+      <c r="G3" s="545"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="542" t="s">
+      <c r="I3" s="546" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="536"/>
-      <c r="K3" s="536"/>
-      <c r="L3" s="537"/>
+      <c r="J3" s="540"/>
+      <c r="K3" s="540"/>
+      <c r="L3" s="541"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="521"/>
-      <c r="O3" s="521"/>
-      <c r="P3" s="503" t="s">
+      <c r="N3" s="511"/>
+      <c r="O3" s="511"/>
+      <c r="P3" s="519" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="504"/>
-      <c r="R3" s="505" t="s">
+      <c r="Q3" s="520"/>
+      <c r="R3" s="521" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="506"/>
+      <c r="S3" s="522"/>
       <c r="T3" s="12"/>
       <c r="U3" s="13"/>
       <c r="V3" s="13"/>
@@ -13558,7 +13952,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="543"/>
+      <c r="I4" s="547"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -13621,8 +14015,8 @@
         <f>I5-L5</f>
         <v>0</v>
       </c>
-      <c r="R5" s="507"/>
-      <c r="S5" s="507"/>
+      <c r="R5" s="523"/>
+      <c r="S5" s="523"/>
       <c r="T5" s="12"/>
       <c r="U5" s="13"/>
       <c r="V5" s="13"/>
@@ -13671,8 +14065,8 @@
         <f>O6-L6</f>
         <v>0</v>
       </c>
-      <c r="R6" s="508"/>
-      <c r="S6" s="508"/>
+      <c r="R6" s="524"/>
+      <c r="S6" s="524"/>
       <c r="T6" s="180"/>
       <c r="U6" s="13"/>
       <c r="V6" s="46"/>
@@ -13763,8 +14157,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R8" s="509"/>
-      <c r="S8" s="509"/>
+      <c r="R8" s="525"/>
+      <c r="S8" s="525"/>
       <c r="T8" s="45"/>
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
@@ -13839,8 +14233,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R10" s="510"/>
-      <c r="S10" s="510"/>
+      <c r="R10" s="526"/>
+      <c r="S10" s="526"/>
       <c r="T10" s="45"/>
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
@@ -13987,8 +14381,8 @@
         <f>O13-I13</f>
         <v>0</v>
       </c>
-      <c r="R13" s="511"/>
-      <c r="S13" s="511"/>
+      <c r="R13" s="527"/>
+      <c r="S13" s="527"/>
       <c r="T13" s="45"/>
       <c r="U13" s="66"/>
       <c r="V13" s="66"/>
@@ -14307,8 +14701,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R20" s="512"/>
-      <c r="S20" s="512"/>
+      <c r="R20" s="528"/>
+      <c r="S20" s="528"/>
       <c r="T20" s="45"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
@@ -14395,8 +14789,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="R22" s="513"/>
-      <c r="S22" s="513"/>
+      <c r="R22" s="529"/>
+      <c r="S22" s="529"/>
       <c r="T22" s="45"/>
       <c r="U22" s="78"/>
       <c r="V22" s="78"/>
@@ -14445,8 +14839,8 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="R23" s="514"/>
-      <c r="S23" s="514"/>
+      <c r="R23" s="530"/>
+      <c r="S23" s="530"/>
       <c r="T23" s="347" t="s">
         <v>99</v>
       </c>
@@ -14597,8 +14991,8 @@
         <f t="shared" si="5"/>
         <v>-1</v>
       </c>
-      <c r="R26" s="515"/>
-      <c r="S26" s="515"/>
+      <c r="R26" s="531"/>
+      <c r="S26" s="531"/>
       <c r="T26" s="347" t="s">
         <v>99</v>
       </c>
@@ -15675,10 +16069,10 @@
     <row r="51" spans="2:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="544" t="s">
+      <c r="F51" s="548" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="544"/>
+      <c r="G51" s="548"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>55132.759999999995</v>
@@ -15906,14 +16300,6 @@
     <sortCondition ref="B27:B47"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
@@ -15926,6 +16312,14 @@
     <mergeCell ref="R22:S22"/>
     <mergeCell ref="R23:S23"/>
     <mergeCell ref="R26:S26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:L3"/>
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15971,10 +16365,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="507"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -15988,30 +16382,30 @@
       <c r="R1" s="13"/>
     </row>
     <row r="2" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="550">
+      <c r="B2" s="554">
         <v>45108</v>
       </c>
-      <c r="C2" s="551"/>
-      <c r="F2" s="530" t="s">
+      <c r="C2" s="555"/>
+      <c r="F2" s="534" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="531"/>
-      <c r="H2" s="532"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="534" t="s">
+      <c r="G2" s="535"/>
+      <c r="H2" s="536"/>
+      <c r="I2" s="537"/>
+      <c r="J2" s="538" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="534"/>
-      <c r="L2" s="535"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="539"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="521" t="s">
+      <c r="N2" s="511" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="521"/>
-      <c r="P2" s="545" t="s">
+      <c r="O2" s="511"/>
+      <c r="P2" s="549" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="546"/>
+      <c r="Q2" s="550"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -16019,27 +16413,27 @@
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="538" t="s">
+      <c r="C3" s="542" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="539"/>
+      <c r="D3" s="543"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="540" t="s">
+      <c r="F3" s="544" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="541"/>
+      <c r="G3" s="545"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="542" t="s">
+      <c r="I3" s="546" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="536"/>
-      <c r="K3" s="536"/>
-      <c r="L3" s="537"/>
+      <c r="J3" s="540"/>
+      <c r="K3" s="540"/>
+      <c r="L3" s="541"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="521"/>
-      <c r="O3" s="521"/>
-      <c r="P3" s="547"/>
-      <c r="Q3" s="548"/>
+      <c r="N3" s="511"/>
+      <c r="O3" s="511"/>
+      <c r="P3" s="551"/>
+      <c r="Q3" s="552"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -16066,7 +16460,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="543"/>
+      <c r="I4" s="547"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -16591,7 +16985,7 @@
         <v>-16</v>
       </c>
       <c r="R15" s="411"/>
-      <c r="S15" s="549" t="s">
+      <c r="S15" s="553" t="s">
         <v>109</v>
       </c>
       <c r="T15" s="13"/>
@@ -16642,7 +17036,7 @@
         <v>6</v>
       </c>
       <c r="R16" s="412"/>
-      <c r="S16" s="549"/>
+      <c r="S16" s="553"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
@@ -18117,10 +18511,10 @@
     <row r="51" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="544" t="s">
+      <c r="F51" s="548" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="544"/>
+      <c r="G51" s="548"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>34034.630000000005</v>
@@ -18363,7 +18757,7 @@
   <dimension ref="A1:Z63"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -18390,10 +18784,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="506" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="507"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -18407,30 +18801,30 @@
       <c r="R1" s="13"/>
     </row>
     <row r="2" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="550">
+      <c r="B2" s="554">
         <v>45136</v>
       </c>
-      <c r="C2" s="551"/>
-      <c r="F2" s="530" t="s">
+      <c r="C2" s="555"/>
+      <c r="F2" s="534" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="531"/>
-      <c r="H2" s="532"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="534" t="s">
+      <c r="G2" s="535"/>
+      <c r="H2" s="536"/>
+      <c r="I2" s="537"/>
+      <c r="J2" s="538" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="534"/>
-      <c r="L2" s="535"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="539"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="552" t="s">
+      <c r="N2" s="556" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="552"/>
-      <c r="P2" s="545" t="s">
+      <c r="O2" s="556"/>
+      <c r="P2" s="549" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="546"/>
+      <c r="Q2" s="550"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -18438,27 +18832,27 @@
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14"/>
-      <c r="C3" s="538" t="s">
+      <c r="C3" s="542" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="539"/>
+      <c r="D3" s="543"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="540" t="s">
+      <c r="F3" s="544" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="541"/>
+      <c r="G3" s="545"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="542" t="s">
+      <c r="I3" s="546" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="536"/>
-      <c r="K3" s="536"/>
-      <c r="L3" s="537"/>
+      <c r="J3" s="540"/>
+      <c r="K3" s="540"/>
+      <c r="L3" s="541"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="552"/>
-      <c r="O3" s="552"/>
-      <c r="P3" s="547"/>
-      <c r="Q3" s="548"/>
+      <c r="N3" s="556"/>
+      <c r="O3" s="556"/>
+      <c r="P3" s="551"/>
+      <c r="Q3" s="552"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -18485,7 +18879,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="543"/>
+      <c r="I4" s="547"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -20440,10 +20834,10 @@
     <row r="51" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="544" t="s">
+      <c r="F51" s="548" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="544"/>
+      <c r="G51" s="548"/>
       <c r="H51" s="148">
         <f>SUM(H5:H34)</f>
         <v>42356.71</v>
@@ -20664,16 +21058,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N2:O3"/>
+    <mergeCell ref="P2:Q3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:I4"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:L3"/>
-    <mergeCell ref="N2:O3"/>
-    <mergeCell ref="P2:Q3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.39" right="0.23622047244094491" top="0.31496062992125984" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" scale="65" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -20688,11 +21082,8 @@
   </sheetPr>
   <dimension ref="A1:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="8" topLeftCell="L9" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -20719,10 +21110,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="516" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="517"/>
+      <c r="B1" s="627" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="627"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -20736,58 +21127,58 @@
       <c r="R1" s="13"/>
     </row>
     <row r="2" spans="2:26" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="550">
+      <c r="B2" s="628">
         <v>45171</v>
       </c>
-      <c r="C2" s="551"/>
-      <c r="F2" s="530" t="s">
+      <c r="C2" s="629"/>
+      <c r="F2" s="534" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="531"/>
-      <c r="H2" s="532"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="534" t="s">
+      <c r="G2" s="535"/>
+      <c r="H2" s="536"/>
+      <c r="I2" s="537"/>
+      <c r="J2" s="538" t="s">
         <v>62</v>
       </c>
-      <c r="K2" s="534"/>
-      <c r="L2" s="535"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="539"/>
       <c r="M2" s="221"/>
-      <c r="N2" s="552" t="s">
+      <c r="N2" s="556" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="552"/>
-      <c r="P2" s="545" t="s">
+      <c r="O2" s="556"/>
+      <c r="P2" s="549" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="546"/>
+      <c r="Q2" s="550"/>
       <c r="S2" s="12"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
       <c r="V2" s="13"/>
     </row>
     <row r="3" spans="2:26" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="14"/>
-      <c r="C3" s="538" t="s">
+      <c r="B3" s="625"/>
+      <c r="C3" s="626" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="539"/>
+      <c r="D3" s="543"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="540" t="s">
+      <c r="F3" s="544" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="541"/>
+      <c r="G3" s="545"/>
       <c r="H3" s="233"/>
-      <c r="I3" s="542" t="s">
+      <c r="I3" s="546" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="536"/>
-      <c r="K3" s="536"/>
-      <c r="L3" s="537"/>
+      <c r="J3" s="540"/>
+      <c r="K3" s="540"/>
+      <c r="L3" s="541"/>
       <c r="M3" s="222"/>
-      <c r="N3" s="552"/>
-      <c r="O3" s="552"/>
-      <c r="P3" s="547"/>
-      <c r="Q3" s="548"/>
+      <c r="N3" s="556"/>
+      <c r="O3" s="556"/>
+      <c r="P3" s="551"/>
+      <c r="Q3" s="552"/>
       <c r="R3" s="434"/>
       <c r="S3" s="12"/>
       <c r="T3" s="13"/>
@@ -20814,7 +21205,7 @@
       <c r="H4" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="543"/>
+      <c r="I4" s="547"/>
       <c r="J4" s="235"/>
       <c r="K4" s="236" t="s">
         <v>7</v>
@@ -20994,7 +21385,7 @@
       <c r="V8" s="13"/>
     </row>
     <row r="9" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="569" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="28"/>
@@ -21022,15 +21413,19 @@
         <v>15</v>
       </c>
       <c r="M9" s="42"/>
-      <c r="N9" s="244"/>
-      <c r="O9" s="245"/>
+      <c r="N9" s="602">
+        <v>464.05</v>
+      </c>
+      <c r="O9" s="603">
+        <v>15</v>
+      </c>
       <c r="P9" s="325">
         <f t="shared" si="1"/>
-        <v>-463.87</v>
+        <v>0.18000000000000682</v>
       </c>
       <c r="Q9" s="326">
         <f t="shared" si="1"/>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="R9" s="57"/>
       <c r="S9" s="45"/>
@@ -21039,7 +21434,7 @@
       <c r="V9" s="13"/>
     </row>
     <row r="10" spans="2:26" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="569" t="s">
         <v>71</v>
       </c>
       <c r="C10" s="28"/>
@@ -21059,8 +21454,8 @@
       <c r="K10" s="279"/>
       <c r="L10" s="214"/>
       <c r="M10" s="42"/>
-      <c r="N10" s="244"/>
-      <c r="O10" s="245"/>
+      <c r="N10" s="602"/>
+      <c r="O10" s="603"/>
       <c r="P10" s="325">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -21076,7 +21471,7 @@
       <c r="V10" s="13"/>
     </row>
     <row r="11" spans="2:26" ht="28.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="569" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="28"/>
@@ -21104,15 +21499,19 @@
         <v>12</v>
       </c>
       <c r="M11" s="42"/>
-      <c r="N11" s="244"/>
-      <c r="O11" s="245"/>
-      <c r="P11" s="325">
+      <c r="N11" s="602">
+        <v>130</v>
+      </c>
+      <c r="O11" s="603">
+        <v>13</v>
+      </c>
+      <c r="P11" s="608">
         <f t="shared" si="1"/>
-        <v>-120</v>
-      </c>
-      <c r="Q11" s="326">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="609">
         <f t="shared" si="1"/>
-        <v>-12</v>
+        <v>1</v>
       </c>
       <c r="R11" s="495"/>
       <c r="S11" s="180"/>
@@ -21121,7 +21520,7 @@
       <c r="V11" s="13"/>
     </row>
     <row r="12" spans="2:26" ht="30" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="569" t="s">
         <v>106</v>
       </c>
       <c r="C12" s="28"/>
@@ -21141,8 +21540,8 @@
       <c r="K12" s="279"/>
       <c r="L12" s="214"/>
       <c r="M12" s="42"/>
-      <c r="N12" s="244"/>
-      <c r="O12" s="245"/>
+      <c r="N12" s="602"/>
+      <c r="O12" s="603"/>
       <c r="P12" s="327">
         <f t="shared" ref="P12:Q50" si="2">H12-K12</f>
         <v>0</v>
@@ -21158,7 +21557,7 @@
       <c r="V12" s="13"/>
     </row>
     <row r="13" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="569" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="28">
@@ -21174,31 +21573,35 @@
       <c r="G13" s="31">
         <v>5</v>
       </c>
-      <c r="H13" s="227">
+      <c r="H13" s="576">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="I13" s="225">
+      <c r="I13" s="577">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="279">
+      <c r="J13" s="578"/>
+      <c r="K13" s="579">
         <v>160</v>
       </c>
-      <c r="L13" s="214">
+      <c r="L13" s="580">
         <v>16</v>
       </c>
-      <c r="M13" s="42"/>
-      <c r="N13" s="244"/>
-      <c r="O13" s="245"/>
+      <c r="M13" s="581"/>
+      <c r="N13" s="602">
+        <v>160</v>
+      </c>
+      <c r="O13" s="603">
+        <v>16</v>
+      </c>
       <c r="P13" s="327">
         <f>N13-H13</f>
-        <v>-160</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="328">
         <f>O13-I13</f>
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="R13" s="496"/>
       <c r="S13" s="422"/>
@@ -21206,8 +21609,8 @@
       <c r="U13" s="66"/>
       <c r="V13" s="13"/>
     </row>
-    <row r="14" spans="2:26" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="30" t="s">
+    <row r="14" spans="2:26" ht="60.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="569" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="60"/>
@@ -21219,42 +21622,46 @@
       <c r="G14" s="31">
         <v>17</v>
       </c>
-      <c r="H14" s="227">
+      <c r="H14" s="576">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="I14" s="225">
+      <c r="I14" s="577">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="J14" s="455"/>
-      <c r="K14" s="372">
+      <c r="J14" s="582"/>
+      <c r="K14" s="583">
         <v>150</v>
       </c>
-      <c r="L14" s="373">
+      <c r="L14" s="584">
         <v>15</v>
       </c>
-      <c r="M14" s="42"/>
-      <c r="N14" s="244"/>
-      <c r="O14" s="245"/>
-      <c r="P14" s="327">
-        <f t="shared" ref="P14:Q39" si="3">N14-H14</f>
-        <v>-170</v>
-      </c>
-      <c r="Q14" s="328">
+      <c r="M14" s="581"/>
+      <c r="N14" s="604">
+        <v>150</v>
+      </c>
+      <c r="O14" s="605">
+        <v>15</v>
+      </c>
+      <c r="P14" s="475">
+        <f t="shared" ref="P14:Q40" si="3">N14-H14</f>
+        <v>-20</v>
+      </c>
+      <c r="Q14" s="476">
         <f t="shared" si="3"/>
-        <v>-17</v>
+        <v>-2</v>
       </c>
       <c r="R14" s="411"/>
-      <c r="S14" s="561" t="s">
-        <v>133</v>
+      <c r="S14" s="610" t="s">
+        <v>137</v>
       </c>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
     </row>
     <row r="15" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="570" t="s">
         <v>75</v>
       </c>
       <c r="C15" s="28"/>
@@ -21266,42 +21673,46 @@
       <c r="G15" s="31">
         <v>2</v>
       </c>
-      <c r="H15" s="458">
+      <c r="H15" s="585">
         <f t="shared" si="0"/>
         <v>63.72</v>
       </c>
-      <c r="I15" s="225">
+      <c r="I15" s="577">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J15" s="455"/>
-      <c r="K15" s="461">
+      <c r="J15" s="582"/>
+      <c r="K15" s="586">
         <v>96.81</v>
       </c>
-      <c r="L15" s="373">
+      <c r="L15" s="584">
         <v>3</v>
       </c>
-      <c r="M15" s="42"/>
-      <c r="N15" s="244"/>
-      <c r="O15" s="245"/>
-      <c r="P15" s="327">
+      <c r="M15" s="581"/>
+      <c r="N15" s="565">
+        <v>96.813999999999993</v>
+      </c>
+      <c r="O15" s="566">
+        <v>3</v>
+      </c>
+      <c r="P15" s="619">
         <f t="shared" si="3"/>
-        <v>-63.72</v>
-      </c>
-      <c r="Q15" s="328">
+        <v>33.093999999999994</v>
+      </c>
+      <c r="Q15" s="448">
         <f t="shared" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="R15" s="411"/>
-      <c r="S15" s="563" t="s">
-        <v>134</v>
+      <c r="S15" s="611" t="s">
+        <v>138</v>
       </c>
       <c r="T15" s="13"/>
       <c r="U15" s="13"/>
       <c r="V15" s="13"/>
     </row>
     <row r="16" spans="2:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="570" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="28"/>
@@ -21313,36 +21724,36 @@
       <c r="G16" s="31">
         <v>0</v>
       </c>
-      <c r="H16" s="458">
+      <c r="H16" s="585">
         <f t="shared" si="0"/>
         <v>33.090000000000003</v>
       </c>
-      <c r="I16" s="225">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="455"/>
-      <c r="K16" s="372"/>
-      <c r="L16" s="373"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="244"/>
-      <c r="O16" s="245"/>
-      <c r="P16" s="327">
+      <c r="I16" s="577">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="582"/>
+      <c r="K16" s="583"/>
+      <c r="L16" s="584"/>
+      <c r="M16" s="581"/>
+      <c r="N16" s="567"/>
+      <c r="O16" s="568"/>
+      <c r="P16" s="619">
         <f t="shared" si="3"/>
         <v>-33.090000000000003</v>
       </c>
-      <c r="Q16" s="328">
+      <c r="Q16" s="448">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R16" s="412"/>
-      <c r="S16" s="564"/>
+      <c r="S16" s="612"/>
       <c r="T16" s="13"/>
       <c r="U16" s="13"/>
       <c r="V16" s="13"/>
     </row>
     <row r="17" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="569" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="28"/>
@@ -21350,79 +21761,79 @@
       <c r="E17" s="30"/>
       <c r="F17" s="28"/>
       <c r="G17" s="31"/>
-      <c r="H17" s="227">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="225">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="54"/>
-      <c r="K17" s="279"/>
-      <c r="L17" s="214"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="244"/>
-      <c r="O17" s="245"/>
-      <c r="P17" s="327">
+      <c r="H17" s="576">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="577">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="578"/>
+      <c r="K17" s="579"/>
+      <c r="L17" s="580"/>
+      <c r="M17" s="581"/>
+      <c r="N17" s="563"/>
+      <c r="O17" s="564"/>
+      <c r="P17" s="620">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="328">
+      <c r="Q17" s="621">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R17" s="412"/>
-      <c r="S17" s="562"/>
+      <c r="S17" s="613"/>
       <c r="T17" s="13"/>
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
     </row>
-    <row r="18" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="30" t="s">
+    <row r="18" spans="2:22" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="557" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="565">
+      <c r="C18" s="559"/>
+      <c r="D18" s="560"/>
+      <c r="E18" s="558"/>
+      <c r="F18" s="561">
         <v>-31.08</v>
       </c>
-      <c r="G18" s="566">
+      <c r="G18" s="562">
         <v>-5</v>
       </c>
-      <c r="H18" s="458">
+      <c r="H18" s="587">
         <f t="shared" si="0"/>
         <v>-31.08</v>
       </c>
-      <c r="I18" s="457">
+      <c r="I18" s="588">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="J18" s="455"/>
-      <c r="K18" s="372"/>
-      <c r="L18" s="373"/>
-      <c r="M18" s="42"/>
+      <c r="J18" s="582"/>
+      <c r="K18" s="583"/>
+      <c r="L18" s="584"/>
+      <c r="M18" s="581"/>
       <c r="N18" s="244"/>
       <c r="O18" s="245"/>
-      <c r="P18" s="327">
+      <c r="P18" s="623">
         <f t="shared" si="3"/>
         <v>31.08</v>
       </c>
-      <c r="Q18" s="328">
+      <c r="Q18" s="624">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="R18" s="436"/>
-      <c r="S18" s="477" t="s">
-        <v>135</v>
+      <c r="S18" s="614" t="s">
+        <v>133</v>
       </c>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
     </row>
     <row r="19" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="569" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="28"/>
@@ -21434,40 +21845,44 @@
       <c r="G19" s="31">
         <v>409</v>
       </c>
-      <c r="H19" s="227">
+      <c r="H19" s="576">
         <f t="shared" si="0"/>
         <v>11894.42</v>
       </c>
-      <c r="I19" s="225">
+      <c r="I19" s="577">
         <f t="shared" si="0"/>
         <v>409</v>
       </c>
-      <c r="J19" s="54"/>
-      <c r="K19" s="279">
+      <c r="J19" s="578"/>
+      <c r="K19" s="579">
         <v>11894.42</v>
       </c>
-      <c r="L19" s="214">
+      <c r="L19" s="580">
         <v>409</v>
       </c>
-      <c r="M19" s="42"/>
-      <c r="N19" s="244"/>
-      <c r="O19" s="245"/>
-      <c r="P19" s="327">
+      <c r="M19" s="581"/>
+      <c r="N19" s="602">
+        <v>11919.06</v>
+      </c>
+      <c r="O19" s="603">
+        <v>410</v>
+      </c>
+      <c r="P19" s="622">
         <f t="shared" si="3"/>
-        <v>-11894.42</v>
-      </c>
-      <c r="Q19" s="328">
+        <v>24.639999999999418</v>
+      </c>
+      <c r="Q19" s="609">
         <f t="shared" si="3"/>
-        <v>-409</v>
+        <v>1</v>
       </c>
       <c r="R19" s="437"/>
-      <c r="S19" s="555"/>
+      <c r="S19" s="502"/>
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
       <c r="V19" s="13"/>
     </row>
     <row r="20" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="569" t="s">
         <v>119</v>
       </c>
       <c r="C20" s="28"/>
@@ -21475,20 +21890,20 @@
       <c r="E20" s="30"/>
       <c r="F20" s="28"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="227">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="225">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="279"/>
-      <c r="L20" s="214"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="244"/>
-      <c r="O20" s="245"/>
+      <c r="H20" s="576">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="577">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="578"/>
+      <c r="K20" s="579"/>
+      <c r="L20" s="580"/>
+      <c r="M20" s="581"/>
+      <c r="N20" s="602"/>
+      <c r="O20" s="603"/>
       <c r="P20" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21504,7 +21919,7 @@
       <c r="V20" s="13"/>
     </row>
     <row r="21" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="569" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="28"/>
@@ -21512,20 +21927,20 @@
       <c r="E21" s="30"/>
       <c r="F21" s="28"/>
       <c r="G21" s="31"/>
-      <c r="H21" s="227">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="225">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="54"/>
-      <c r="K21" s="279"/>
-      <c r="L21" s="214"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="244"/>
-      <c r="O21" s="245"/>
+      <c r="H21" s="576">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="577">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="578"/>
+      <c r="K21" s="579"/>
+      <c r="L21" s="580"/>
+      <c r="M21" s="581"/>
+      <c r="N21" s="602"/>
+      <c r="O21" s="603"/>
       <c r="P21" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21541,7 +21956,7 @@
       <c r="V21" s="13"/>
     </row>
     <row r="22" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="569" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="28"/>
@@ -21549,20 +21964,20 @@
       <c r="E22" s="30"/>
       <c r="F22" s="28"/>
       <c r="G22" s="31"/>
-      <c r="H22" s="227">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="225">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="54"/>
-      <c r="K22" s="279"/>
-      <c r="L22" s="214"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="244"/>
-      <c r="O22" s="245"/>
+      <c r="H22" s="576">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="577">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="578"/>
+      <c r="K22" s="579"/>
+      <c r="L22" s="580"/>
+      <c r="M22" s="581"/>
+      <c r="N22" s="602"/>
+      <c r="O22" s="603"/>
       <c r="P22" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21578,7 +21993,7 @@
       <c r="V22" s="13"/>
     </row>
     <row r="23" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="569" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="28">
@@ -21594,31 +22009,35 @@
       <c r="G23" s="31">
         <v>111</v>
       </c>
-      <c r="H23" s="227">
+      <c r="H23" s="576">
         <f t="shared" si="0"/>
         <v>2366.5</v>
       </c>
-      <c r="I23" s="225">
+      <c r="I23" s="577">
         <f t="shared" si="0"/>
         <v>131</v>
       </c>
-      <c r="J23" s="54"/>
-      <c r="K23" s="279">
+      <c r="J23" s="578"/>
+      <c r="K23" s="579">
         <v>2366.5</v>
       </c>
-      <c r="L23" s="214">
+      <c r="L23" s="580">
         <v>131</v>
       </c>
-      <c r="M23" s="42"/>
-      <c r="N23" s="244"/>
-      <c r="O23" s="245"/>
+      <c r="M23" s="581"/>
+      <c r="N23" s="602">
+        <v>2366.5</v>
+      </c>
+      <c r="O23" s="603">
+        <v>131</v>
+      </c>
       <c r="P23" s="327">
         <f t="shared" si="3"/>
-        <v>-2366.5</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="328">
         <f t="shared" si="3"/>
-        <v>-131</v>
+        <v>0</v>
       </c>
       <c r="R23" s="499"/>
       <c r="S23" s="426"/>
@@ -21627,7 +22046,7 @@
       <c r="V23" s="13"/>
     </row>
     <row r="24" spans="2:22" ht="29.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="569" t="s">
         <v>94</v>
       </c>
       <c r="C24" s="28"/>
@@ -21635,20 +22054,20 @@
       <c r="E24" s="30"/>
       <c r="F24" s="28"/>
       <c r="G24" s="31"/>
-      <c r="H24" s="227">
+      <c r="H24" s="576">
         <f t="shared" ref="H24:I47" si="4">F24+C24</f>
         <v>0</v>
       </c>
-      <c r="I24" s="225">
+      <c r="I24" s="577">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J24" s="54"/>
-      <c r="K24" s="279"/>
-      <c r="L24" s="214"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="244"/>
-      <c r="O24" s="245"/>
+      <c r="J24" s="578"/>
+      <c r="K24" s="579"/>
+      <c r="L24" s="580"/>
+      <c r="M24" s="581"/>
+      <c r="N24" s="602"/>
+      <c r="O24" s="603"/>
       <c r="P24" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21663,8 +22082,8 @@
       <c r="U24" s="13"/>
       <c r="V24" s="13"/>
     </row>
-    <row r="25" spans="2:22" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="30" t="s">
+    <row r="25" spans="2:22" ht="55.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="569" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="28"/>
@@ -21676,42 +22095,46 @@
       <c r="G25" s="31">
         <v>676</v>
       </c>
-      <c r="H25" s="458">
+      <c r="H25" s="585">
         <f t="shared" si="4"/>
         <v>3069.04</v>
       </c>
-      <c r="I25" s="457">
+      <c r="I25" s="589">
         <f t="shared" si="4"/>
         <v>676</v>
       </c>
-      <c r="J25" s="455"/>
-      <c r="K25" s="372">
+      <c r="J25" s="582"/>
+      <c r="K25" s="583">
         <v>3073.58</v>
       </c>
-      <c r="L25" s="373">
+      <c r="L25" s="584">
         <v>677</v>
       </c>
-      <c r="M25" s="42"/>
-      <c r="N25" s="244"/>
-      <c r="O25" s="245"/>
+      <c r="M25" s="581"/>
+      <c r="N25" s="602">
+        <v>3073.58</v>
+      </c>
+      <c r="O25" s="603">
+        <v>677</v>
+      </c>
       <c r="P25" s="327">
         <f t="shared" si="3"/>
-        <v>-3069.04</v>
+        <v>4.5399999999999636</v>
       </c>
       <c r="Q25" s="328">
         <f t="shared" si="3"/>
-        <v>-676</v>
+        <v>1</v>
       </c>
       <c r="R25" s="438"/>
-      <c r="S25" s="567" t="s">
-        <v>136</v>
+      <c r="S25" s="615" t="s">
+        <v>134</v>
       </c>
       <c r="T25" s="13"/>
       <c r="U25" s="13"/>
       <c r="V25" s="13"/>
     </row>
     <row r="26" spans="2:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="569" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="28"/>
@@ -21723,31 +22146,35 @@
       <c r="G26" s="31">
         <v>27</v>
       </c>
-      <c r="H26" s="227">
+      <c r="H26" s="576">
         <f t="shared" si="4"/>
         <v>726.99</v>
       </c>
-      <c r="I26" s="225">
+      <c r="I26" s="577">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="J26" s="54"/>
-      <c r="K26" s="279">
+      <c r="J26" s="578"/>
+      <c r="K26" s="579">
         <v>727.04</v>
       </c>
-      <c r="L26" s="214">
+      <c r="L26" s="580">
         <v>27</v>
       </c>
-      <c r="M26" s="42"/>
-      <c r="N26" s="244"/>
-      <c r="O26" s="245"/>
+      <c r="M26" s="581"/>
+      <c r="N26" s="602">
+        <v>727.33</v>
+      </c>
+      <c r="O26" s="603">
+        <v>27</v>
+      </c>
       <c r="P26" s="327">
         <f t="shared" si="3"/>
-        <v>-726.99</v>
+        <v>0.34000000000003183</v>
       </c>
       <c r="Q26" s="328">
         <f t="shared" si="3"/>
-        <v>-27</v>
+        <v>0</v>
       </c>
       <c r="R26" s="500"/>
       <c r="S26" s="426"/>
@@ -21756,7 +22183,7 @@
       <c r="V26" s="13"/>
     </row>
     <row r="27" spans="2:22" ht="29.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="569" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="28"/>
@@ -21764,20 +22191,20 @@
       <c r="E27" s="30"/>
       <c r="F27" s="87"/>
       <c r="G27" s="88"/>
-      <c r="H27" s="227">
+      <c r="H27" s="576">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I27" s="225">
+      <c r="I27" s="577">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J27" s="54"/>
-      <c r="K27" s="279"/>
-      <c r="L27" s="214"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="244"/>
-      <c r="O27" s="245"/>
+      <c r="J27" s="578"/>
+      <c r="K27" s="579"/>
+      <c r="L27" s="580"/>
+      <c r="M27" s="581"/>
+      <c r="N27" s="602"/>
+      <c r="O27" s="603"/>
       <c r="P27" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21793,7 +22220,7 @@
       <c r="V27" s="13"/>
     </row>
     <row r="28" spans="2:22" ht="29.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="64" t="s">
+      <c r="B28" s="570" t="s">
         <v>33</v>
       </c>
       <c r="C28" s="28"/>
@@ -21801,20 +22228,20 @@
       <c r="E28" s="30"/>
       <c r="F28" s="87"/>
       <c r="G28" s="88"/>
-      <c r="H28" s="227">
+      <c r="H28" s="576">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I28" s="225">
+      <c r="I28" s="577">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J28" s="54"/>
-      <c r="K28" s="279"/>
-      <c r="L28" s="214"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="244"/>
-      <c r="O28" s="245"/>
+      <c r="J28" s="578"/>
+      <c r="K28" s="579"/>
+      <c r="L28" s="580"/>
+      <c r="M28" s="581"/>
+      <c r="N28" s="602"/>
+      <c r="O28" s="603"/>
       <c r="P28" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21830,7 +22257,7 @@
       <c r="V28" s="13"/>
     </row>
     <row r="29" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="569" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="28"/>
@@ -21838,20 +22265,20 @@
       <c r="E29" s="30"/>
       <c r="F29" s="87"/>
       <c r="G29" s="88"/>
-      <c r="H29" s="227">
+      <c r="H29" s="576">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I29" s="225">
+      <c r="I29" s="577">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="279"/>
-      <c r="L29" s="214"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="244"/>
-      <c r="O29" s="245"/>
+      <c r="J29" s="578"/>
+      <c r="K29" s="579"/>
+      <c r="L29" s="580"/>
+      <c r="M29" s="581"/>
+      <c r="N29" s="602"/>
+      <c r="O29" s="603"/>
       <c r="P29" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21867,7 +22294,7 @@
       <c r="V29" s="13"/>
     </row>
     <row r="30" spans="2:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="569" t="s">
         <v>70</v>
       </c>
       <c r="C30" s="28"/>
@@ -21875,20 +22302,20 @@
       <c r="E30" s="30"/>
       <c r="F30" s="87"/>
       <c r="G30" s="88"/>
-      <c r="H30" s="227">
+      <c r="H30" s="576">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I30" s="225">
+      <c r="I30" s="577">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J30" s="54"/>
-      <c r="K30" s="279"/>
-      <c r="L30" s="214"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="244"/>
-      <c r="O30" s="245"/>
+      <c r="J30" s="578"/>
+      <c r="K30" s="579"/>
+      <c r="L30" s="580"/>
+      <c r="M30" s="581"/>
+      <c r="N30" s="602"/>
+      <c r="O30" s="603"/>
       <c r="P30" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -21904,7 +22331,7 @@
       <c r="V30" s="13"/>
     </row>
     <row r="31" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="569" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="28"/>
@@ -21916,40 +22343,44 @@
       <c r="G31" s="88">
         <v>657</v>
       </c>
-      <c r="H31" s="226">
+      <c r="H31" s="590">
         <f t="shared" si="4"/>
         <v>17867.02</v>
       </c>
-      <c r="I31" s="228">
+      <c r="I31" s="591">
         <f t="shared" si="4"/>
         <v>657</v>
       </c>
-      <c r="J31" s="54"/>
-      <c r="K31" s="279">
+      <c r="J31" s="578"/>
+      <c r="K31" s="579">
         <v>17867.02</v>
       </c>
-      <c r="L31" s="214">
+      <c r="L31" s="580">
         <v>657</v>
       </c>
-      <c r="M31" s="42"/>
-      <c r="N31" s="244"/>
-      <c r="O31" s="245"/>
-      <c r="P31" s="327">
+      <c r="M31" s="581"/>
+      <c r="N31" s="602">
+        <v>17883.54</v>
+      </c>
+      <c r="O31" s="603">
+        <v>657</v>
+      </c>
+      <c r="P31" s="475">
         <f t="shared" si="3"/>
-        <v>-17867.02</v>
-      </c>
-      <c r="Q31" s="328">
+        <v>16.520000000000437</v>
+      </c>
+      <c r="Q31" s="476">
         <f t="shared" si="3"/>
-        <v>-657</v>
+        <v>0</v>
       </c>
       <c r="R31" s="496"/>
-      <c r="S31" s="555"/>
+      <c r="S31" s="502"/>
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
     </row>
     <row r="32" spans="2:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="569" t="s">
         <v>120</v>
       </c>
       <c r="C32" s="28">
@@ -21961,29 +22392,33 @@
       <c r="E32" s="30"/>
       <c r="F32" s="87"/>
       <c r="G32" s="88"/>
-      <c r="H32" s="226">
+      <c r="H32" s="590">
         <v>390</v>
       </c>
-      <c r="I32" s="228">
+      <c r="I32" s="591">
         <v>39</v>
       </c>
-      <c r="J32" s="54"/>
-      <c r="K32" s="279">
+      <c r="J32" s="578"/>
+      <c r="K32" s="579">
         <v>390</v>
       </c>
-      <c r="L32" s="214">
+      <c r="L32" s="580">
         <v>39</v>
       </c>
-      <c r="M32" s="42"/>
-      <c r="N32" s="244"/>
-      <c r="O32" s="245"/>
+      <c r="M32" s="581"/>
+      <c r="N32" s="602">
+        <v>370</v>
+      </c>
+      <c r="O32" s="603">
+        <v>37</v>
+      </c>
       <c r="P32" s="327">
         <f t="shared" si="3"/>
-        <v>-390</v>
+        <v>-20</v>
       </c>
       <c r="Q32" s="328">
         <f t="shared" si="3"/>
-        <v>-39</v>
+        <v>-2</v>
       </c>
       <c r="R32" s="496"/>
       <c r="S32" s="422"/>
@@ -21992,7 +22427,7 @@
       <c r="V32" s="13"/>
     </row>
     <row r="33" spans="1:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="569" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="28">
@@ -22004,31 +22439,35 @@
       <c r="E33" s="30"/>
       <c r="F33" s="87"/>
       <c r="G33" s="88"/>
-      <c r="H33" s="226">
+      <c r="H33" s="590">
         <f t="shared" si="4"/>
         <v>11810</v>
       </c>
-      <c r="I33" s="228">
+      <c r="I33" s="591">
         <f t="shared" si="4"/>
         <v>1181</v>
       </c>
-      <c r="J33" s="54"/>
-      <c r="K33" s="279">
+      <c r="J33" s="578"/>
+      <c r="K33" s="579">
         <v>11810</v>
       </c>
-      <c r="L33" s="214">
+      <c r="L33" s="580">
         <v>1181</v>
       </c>
-      <c r="M33" s="42"/>
-      <c r="N33" s="244"/>
-      <c r="O33" s="245"/>
-      <c r="P33" s="327">
+      <c r="M33" s="581"/>
+      <c r="N33" s="602">
+        <v>11820</v>
+      </c>
+      <c r="O33" s="603">
+        <v>1182</v>
+      </c>
+      <c r="P33" s="475">
         <f t="shared" si="3"/>
-        <v>-11810</v>
-      </c>
-      <c r="Q33" s="328">
+        <v>10</v>
+      </c>
+      <c r="Q33" s="476">
         <f t="shared" si="3"/>
-        <v>-1181</v>
+        <v>1</v>
       </c>
       <c r="R33" s="416"/>
       <c r="S33" s="422"/>
@@ -22037,7 +22476,7 @@
       <c r="V33" s="13"/>
     </row>
     <row r="34" spans="1:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="558" t="s">
+      <c r="B34" s="571" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="96">
@@ -22049,31 +22488,35 @@
       <c r="E34" s="98"/>
       <c r="F34" s="96"/>
       <c r="G34" s="103"/>
-      <c r="H34" s="226">
+      <c r="H34" s="590">
         <f t="shared" si="4"/>
         <v>2570</v>
       </c>
-      <c r="I34" s="228">
+      <c r="I34" s="591">
         <f t="shared" si="4"/>
         <v>257</v>
       </c>
-      <c r="J34" s="54"/>
-      <c r="K34" s="279">
+      <c r="J34" s="578"/>
+      <c r="K34" s="579">
         <v>2570</v>
       </c>
-      <c r="L34" s="214">
+      <c r="L34" s="580">
         <v>257</v>
       </c>
-      <c r="M34" s="42"/>
-      <c r="N34" s="244"/>
-      <c r="O34" s="245"/>
+      <c r="M34" s="581"/>
+      <c r="N34" s="602">
+        <v>2570</v>
+      </c>
+      <c r="O34" s="603">
+        <v>57</v>
+      </c>
       <c r="P34" s="327">
         <f t="shared" si="3"/>
-        <v>-2570</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="328">
         <f t="shared" si="3"/>
-        <v>-257</v>
+        <v>-200</v>
       </c>
       <c r="R34" s="417"/>
       <c r="S34" s="422"/>
@@ -22082,7 +22525,7 @@
       <c r="V34" s="13"/>
     </row>
     <row r="35" spans="1:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="102" t="s">
+      <c r="B35" s="186" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="96"/>
@@ -22090,20 +22533,20 @@
       <c r="E35" s="102"/>
       <c r="F35" s="96"/>
       <c r="G35" s="103"/>
-      <c r="H35" s="226">
+      <c r="H35" s="590">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I35" s="228">
+      <c r="I35" s="591">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J35" s="54"/>
-      <c r="K35" s="279"/>
-      <c r="L35" s="214"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="244"/>
-      <c r="O35" s="245"/>
+      <c r="J35" s="578"/>
+      <c r="K35" s="579"/>
+      <c r="L35" s="580"/>
+      <c r="M35" s="581"/>
+      <c r="N35" s="602"/>
+      <c r="O35" s="603"/>
       <c r="P35" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22119,7 +22562,7 @@
       <c r="V35" s="13"/>
     </row>
     <row r="36" spans="1:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="102" t="s">
+      <c r="B36" s="186" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="96"/>
@@ -22127,20 +22570,20 @@
       <c r="E36" s="102"/>
       <c r="F36" s="96"/>
       <c r="G36" s="103"/>
-      <c r="H36" s="226">
+      <c r="H36" s="590">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I36" s="228">
+      <c r="I36" s="591">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J36" s="54"/>
-      <c r="K36" s="279"/>
-      <c r="L36" s="214"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="244"/>
-      <c r="O36" s="245"/>
+      <c r="J36" s="578"/>
+      <c r="K36" s="579"/>
+      <c r="L36" s="580"/>
+      <c r="M36" s="581"/>
+      <c r="N36" s="602"/>
+      <c r="O36" s="603"/>
       <c r="P36" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22156,7 +22599,7 @@
       <c r="V36" s="13"/>
     </row>
     <row r="37" spans="1:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="110" t="s">
+      <c r="B37" s="572" t="s">
         <v>132</v>
       </c>
       <c r="C37" s="28"/>
@@ -22168,31 +22611,35 @@
       <c r="G37" s="103">
         <v>27</v>
       </c>
-      <c r="H37" s="226">
+      <c r="H37" s="590">
         <f t="shared" si="4"/>
         <v>405</v>
       </c>
-      <c r="I37" s="228">
+      <c r="I37" s="591">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="J37" s="54"/>
-      <c r="K37" s="279">
+      <c r="J37" s="578"/>
+      <c r="K37" s="579">
         <v>405</v>
       </c>
-      <c r="L37" s="214">
+      <c r="L37" s="580">
         <v>27</v>
       </c>
-      <c r="M37" s="42"/>
-      <c r="N37" s="244"/>
-      <c r="O37" s="245"/>
+      <c r="M37" s="581"/>
+      <c r="N37" s="602">
+        <v>375</v>
+      </c>
+      <c r="O37" s="603">
+        <v>25</v>
+      </c>
       <c r="P37" s="327">
         <f t="shared" si="3"/>
-        <v>-405</v>
+        <v>-30</v>
       </c>
       <c r="Q37" s="328">
         <f t="shared" si="3"/>
-        <v>-27</v>
+        <v>-2</v>
       </c>
       <c r="R37" s="498"/>
       <c r="S37" s="422"/>
@@ -22202,7 +22649,7 @@
     </row>
     <row r="38" spans="1:22" ht="29.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="109"/>
-      <c r="B38" s="344" t="s">
+      <c r="B38" s="573" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="28"/>
@@ -22210,20 +22657,20 @@
       <c r="E38" s="102"/>
       <c r="F38" s="96"/>
       <c r="G38" s="103"/>
-      <c r="H38" s="226">
+      <c r="H38" s="590">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I38" s="228">
+      <c r="I38" s="591">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J38" s="54"/>
-      <c r="K38" s="279"/>
-      <c r="L38" s="214"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="244"/>
-      <c r="O38" s="245"/>
+      <c r="J38" s="578"/>
+      <c r="K38" s="579"/>
+      <c r="L38" s="580"/>
+      <c r="M38" s="581"/>
+      <c r="N38" s="602"/>
+      <c r="O38" s="603"/>
       <c r="P38" s="327">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -22239,7 +22686,7 @@
       <c r="V38" s="13"/>
     </row>
     <row r="39" spans="1:22" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="557" t="s">
+      <c r="B39" s="504" t="s">
         <v>130</v>
       </c>
       <c r="C39" s="28"/>
@@ -22251,40 +22698,40 @@
       <c r="G39" s="103">
         <v>7</v>
       </c>
-      <c r="H39" s="229">
+      <c r="H39" s="592">
         <f t="shared" si="4"/>
         <v>6327.6</v>
       </c>
-      <c r="I39" s="230">
+      <c r="I39" s="593">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="J39" s="54"/>
-      <c r="K39" s="279">
+      <c r="J39" s="578"/>
+      <c r="K39" s="579">
         <v>6327.6</v>
       </c>
-      <c r="L39" s="214">
+      <c r="L39" s="580">
         <v>7</v>
       </c>
-      <c r="M39" s="42"/>
-      <c r="N39" s="553"/>
-      <c r="O39" s="554"/>
-      <c r="P39" s="327">
+      <c r="M39" s="581"/>
+      <c r="N39" s="606"/>
+      <c r="O39" s="607"/>
+      <c r="P39" s="475">
         <f t="shared" si="3"/>
         <v>-6327.6</v>
       </c>
-      <c r="Q39" s="328">
+      <c r="Q39" s="476">
         <f t="shared" si="3"/>
         <v>-7</v>
       </c>
       <c r="R39" s="114"/>
-      <c r="S39" s="556"/>
+      <c r="S39" s="503"/>
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
       <c r="V39" s="13"/>
     </row>
     <row r="40" spans="1:22" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="560" t="s">
+      <c r="B40" s="505" t="s">
         <v>131</v>
       </c>
       <c r="C40" s="115"/>
@@ -22296,31 +22743,31 @@
       <c r="G40" s="103">
         <v>45</v>
       </c>
-      <c r="H40" s="229">
+      <c r="H40" s="592">
         <f t="shared" si="4"/>
         <v>40710</v>
       </c>
-      <c r="I40" s="230">
+      <c r="I40" s="593">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="J40" s="54"/>
-      <c r="K40" s="279">
+      <c r="J40" s="578"/>
+      <c r="K40" s="579">
         <v>40710</v>
       </c>
-      <c r="L40" s="214">
+      <c r="L40" s="580">
         <v>45</v>
       </c>
-      <c r="M40" s="42"/>
-      <c r="N40" s="244"/>
-      <c r="O40" s="245"/>
-      <c r="P40" s="327">
-        <f t="shared" ref="P40:Q44" si="5">H40-K40</f>
-        <v>0</v>
-      </c>
-      <c r="Q40" s="328">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="M40" s="581"/>
+      <c r="N40" s="602"/>
+      <c r="O40" s="603"/>
+      <c r="P40" s="475">
+        <f t="shared" si="3"/>
+        <v>-40710</v>
+      </c>
+      <c r="Q40" s="476">
+        <f t="shared" si="3"/>
+        <v>-45</v>
       </c>
       <c r="R40" s="419"/>
       <c r="S40" s="432"/>
@@ -22329,7 +22776,7 @@
       <c r="V40" s="13"/>
     </row>
     <row r="41" spans="1:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="263" t="s">
+      <c r="B41" s="574" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="255"/>
@@ -22337,22 +22784,22 @@
       <c r="E41" s="102"/>
       <c r="F41" s="96"/>
       <c r="G41" s="258"/>
-      <c r="H41" s="257">
+      <c r="H41" s="594">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I41" s="230">
+      <c r="I41" s="593">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J41" s="54"/>
-      <c r="K41" s="280"/>
-      <c r="L41" s="256"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="244"/>
-      <c r="O41" s="245"/>
+      <c r="J41" s="578"/>
+      <c r="K41" s="595"/>
+      <c r="L41" s="596"/>
+      <c r="M41" s="581"/>
+      <c r="N41" s="602"/>
+      <c r="O41" s="603"/>
       <c r="P41" s="327">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="P40:Q44" si="5">H41-K41</f>
         <v>0</v>
       </c>
       <c r="Q41" s="328">
@@ -22366,7 +22813,7 @@
       <c r="V41" s="13"/>
     </row>
     <row r="42" spans="1:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="263" t="s">
+      <c r="B42" s="574" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="255"/>
@@ -22374,20 +22821,20 @@
       <c r="E42" s="111"/>
       <c r="F42" s="96"/>
       <c r="G42" s="258"/>
-      <c r="H42" s="257">
+      <c r="H42" s="594">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I42" s="230">
+      <c r="I42" s="593">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J42" s="124"/>
-      <c r="K42" s="281"/>
-      <c r="L42" s="216"/>
-      <c r="M42" s="124"/>
-      <c r="N42" s="244"/>
-      <c r="O42" s="245"/>
+      <c r="J42" s="597"/>
+      <c r="K42" s="598"/>
+      <c r="L42" s="599"/>
+      <c r="M42" s="597"/>
+      <c r="N42" s="602"/>
+      <c r="O42" s="603"/>
       <c r="P42" s="327">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -22403,7 +22850,7 @@
       <c r="V42" s="13"/>
     </row>
     <row r="43" spans="1:22" ht="32.25" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="559" t="s">
+      <c r="B43" s="575" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="115"/>
@@ -22411,20 +22858,20 @@
       <c r="E43" s="30"/>
       <c r="F43" s="28"/>
       <c r="G43" s="259"/>
-      <c r="H43" s="257">
+      <c r="H43" s="594">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I43" s="230">
+      <c r="I43" s="593">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J43" s="54"/>
-      <c r="K43" s="281"/>
-      <c r="L43" s="216"/>
-      <c r="M43" s="124"/>
-      <c r="N43" s="244"/>
-      <c r="O43" s="245"/>
+      <c r="J43" s="578"/>
+      <c r="K43" s="598"/>
+      <c r="L43" s="599"/>
+      <c r="M43" s="597"/>
+      <c r="N43" s="602"/>
+      <c r="O43" s="603"/>
       <c r="P43" s="327">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -22439,8 +22886,8 @@
       <c r="U43" s="13"/>
       <c r="V43" s="13"/>
     </row>
-    <row r="44" spans="1:22" ht="18.75" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="324" t="s">
+    <row r="44" spans="1:22" ht="20.25" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="575" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="115"/>
@@ -22448,20 +22895,20 @@
       <c r="E44" s="30"/>
       <c r="F44" s="28"/>
       <c r="G44" s="259"/>
-      <c r="H44" s="257">
+      <c r="H44" s="594">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I44" s="230">
+      <c r="I44" s="593">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J44" s="54"/>
-      <c r="K44" s="281"/>
-      <c r="L44" s="216"/>
-      <c r="M44" s="124"/>
-      <c r="N44" s="244"/>
-      <c r="O44" s="245"/>
+      <c r="J44" s="578"/>
+      <c r="K44" s="598"/>
+      <c r="L44" s="599"/>
+      <c r="M44" s="597"/>
+      <c r="N44" s="602"/>
+      <c r="O44" s="603"/>
       <c r="P44" s="327">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -22477,7 +22924,7 @@
       <c r="V44" s="13"/>
     </row>
     <row r="45" spans="1:22" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="263" t="s">
+      <c r="B45" s="574" t="s">
         <v>74</v>
       </c>
       <c r="C45" s="115"/>
@@ -22489,31 +22936,35 @@
       <c r="G45" s="259">
         <v>31</v>
       </c>
-      <c r="H45" s="257">
+      <c r="H45" s="594">
         <f t="shared" si="4"/>
         <v>745.85</v>
       </c>
-      <c r="I45" s="230">
+      <c r="I45" s="593">
         <f t="shared" si="4"/>
         <v>31</v>
       </c>
-      <c r="J45" s="54"/>
-      <c r="K45" s="281">
+      <c r="J45" s="578"/>
+      <c r="K45" s="598">
         <v>745.85</v>
       </c>
-      <c r="L45" s="216">
+      <c r="L45" s="599">
         <v>31</v>
       </c>
-      <c r="M45" s="124"/>
-      <c r="N45" s="244"/>
-      <c r="O45" s="245"/>
+      <c r="M45" s="597"/>
+      <c r="N45" s="602">
+        <v>745.87</v>
+      </c>
+      <c r="O45" s="603">
+        <v>36</v>
+      </c>
       <c r="P45" s="327">
         <f>N45-H45</f>
-        <v>-745.85</v>
-      </c>
-      <c r="Q45" s="328">
+        <v>1.999999999998181E-2</v>
+      </c>
+      <c r="Q45" s="476">
         <f>O45-I45</f>
-        <v>-31</v>
+        <v>5</v>
       </c>
       <c r="R45" s="498"/>
       <c r="S45" s="422"/>
@@ -22522,7 +22973,7 @@
       <c r="V45" s="13"/>
     </row>
     <row r="46" spans="1:22" ht="45.75" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="263" t="s">
+      <c r="B46" s="574" t="s">
         <v>60</v>
       </c>
       <c r="C46" s="375"/>
@@ -22530,20 +22981,20 @@
       <c r="E46" s="30"/>
       <c r="F46" s="28"/>
       <c r="G46" s="259"/>
-      <c r="H46" s="449">
+      <c r="H46" s="594">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I46" s="450">
+      <c r="I46" s="600">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J46" s="54"/>
-      <c r="K46" s="281"/>
-      <c r="L46" s="445"/>
-      <c r="M46" s="124"/>
-      <c r="N46" s="244"/>
-      <c r="O46" s="245"/>
+      <c r="J46" s="578"/>
+      <c r="K46" s="598"/>
+      <c r="L46" s="601"/>
+      <c r="M46" s="597"/>
+      <c r="N46" s="602"/>
+      <c r="O46" s="603"/>
       <c r="P46" s="327">
         <f t="shared" ref="P46:Q47" si="6">N46-H46</f>
         <v>0</v>
@@ -22559,7 +23010,7 @@
       <c r="V46" s="13"/>
     </row>
     <row r="47" spans="1:22" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="263" t="s">
+      <c r="B47" s="574" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="115"/>
@@ -22571,31 +23022,35 @@
       <c r="G47" s="259">
         <v>72</v>
       </c>
-      <c r="H47" s="257">
+      <c r="H47" s="594">
         <f t="shared" si="4"/>
         <v>1633.24</v>
       </c>
-      <c r="I47" s="230">
+      <c r="I47" s="593">
         <f t="shared" si="4"/>
         <v>72</v>
       </c>
-      <c r="J47" s="54"/>
-      <c r="K47" s="281">
+      <c r="J47" s="578"/>
+      <c r="K47" s="598">
         <v>1633.24</v>
       </c>
-      <c r="L47" s="216">
+      <c r="L47" s="599">
         <v>72</v>
       </c>
-      <c r="M47" s="124"/>
-      <c r="N47" s="244"/>
-      <c r="O47" s="245"/>
+      <c r="M47" s="597"/>
+      <c r="N47" s="602">
+        <v>1633.26</v>
+      </c>
+      <c r="O47" s="603">
+        <v>72</v>
+      </c>
       <c r="P47" s="327">
         <f t="shared" si="6"/>
-        <v>-1633.24</v>
+        <v>1.999999999998181E-2</v>
       </c>
       <c r="Q47" s="328">
         <f t="shared" si="6"/>
-        <v>-72</v>
+        <v>0</v>
       </c>
       <c r="R47" s="498"/>
       <c r="S47" s="422"/>
@@ -22612,18 +23067,18 @@
       <c r="E48" s="442"/>
       <c r="F48" s="443"/>
       <c r="G48" s="444"/>
-      <c r="H48" s="257">
+      <c r="H48" s="594">
         <f t="shared" ref="H48:I50" si="7">F48+C48</f>
         <v>0</v>
       </c>
-      <c r="I48" s="230">
+      <c r="I48" s="593">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J48" s="54"/>
-      <c r="K48" s="281"/>
-      <c r="L48" s="216"/>
-      <c r="M48" s="124"/>
+      <c r="J48" s="578"/>
+      <c r="K48" s="598"/>
+      <c r="L48" s="599"/>
+      <c r="M48" s="597"/>
       <c r="N48" s="244"/>
       <c r="O48" s="245"/>
       <c r="P48" s="327">
@@ -22647,18 +23102,18 @@
       <c r="E49" s="30"/>
       <c r="F49" s="28"/>
       <c r="G49" s="259"/>
-      <c r="H49" s="257">
+      <c r="H49" s="594">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I49" s="230">
+      <c r="I49" s="593">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J49" s="54"/>
-      <c r="K49" s="281"/>
-      <c r="L49" s="216"/>
-      <c r="M49" s="124"/>
+      <c r="J49" s="578"/>
+      <c r="K49" s="598"/>
+      <c r="L49" s="599"/>
+      <c r="M49" s="597"/>
       <c r="N49" s="244"/>
       <c r="O49" s="245"/>
       <c r="P49" s="327">
@@ -22682,18 +23137,18 @@
       <c r="E50" s="273"/>
       <c r="F50" s="275"/>
       <c r="G50" s="277"/>
-      <c r="H50" s="257">
+      <c r="H50" s="594">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I50" s="230">
+      <c r="I50" s="593">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J50" s="54"/>
-      <c r="K50" s="281"/>
-      <c r="L50" s="216"/>
-      <c r="M50" s="124"/>
+      <c r="J50" s="578"/>
+      <c r="K50" s="598"/>
+      <c r="L50" s="599"/>
+      <c r="M50" s="597"/>
       <c r="N50" s="246"/>
       <c r="O50" s="247"/>
       <c r="P50" s="329">
@@ -22710,18 +23165,18 @@
       <c r="U50" s="13"/>
       <c r="V50" s="13"/>
     </row>
-    <row r="51" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:22" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="145"/>
       <c r="D51" s="147"/>
-      <c r="F51" s="544" t="s">
+      <c r="F51" s="548" t="s">
         <v>46</v>
       </c>
-      <c r="G51" s="544"/>
-      <c r="H51" s="148">
+      <c r="G51" s="548"/>
+      <c r="H51" s="617">
         <f>SUM(H5:H34)</f>
         <v>51673.75</v>
       </c>
-      <c r="I51" s="149">
+      <c r="I51" s="618">
         <f>SUM(I5:I34)</f>
         <v>3434</v>
       </c>
@@ -22729,12 +23184,13 @@
       <c r="K51" s="149"/>
       <c r="L51" s="149"/>
       <c r="M51" s="150"/>
-      <c r="N51" s="151">
+      <c r="N51" s="616">
         <f>SUM(N5:N42)</f>
-        <v>0</v>
-      </c>
-      <c r="O51" s="152" t="s">
-        <v>47</v>
+        <v>52105.874000000003</v>
+      </c>
+      <c r="O51" s="616">
+        <f>SUM(O5:O42)</f>
+        <v>3265</v>
       </c>
       <c r="P51" s="153"/>
       <c r="Q51" s="154"/>
@@ -22806,15 +23262,17 @@
     </row>
     <row r="56" spans="2:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="175"/>
-      <c r="C56" s="482"/>
-      <c r="D56" s="483"/>
-      <c r="E56" s="484"/>
-      <c r="F56" s="484"/>
-      <c r="G56" s="484"/>
-      <c r="H56" s="484"/>
-      <c r="I56" s="484"/>
-      <c r="J56" s="484"/>
-      <c r="K56" s="484"/>
+      <c r="C56" s="350" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="163"/>
+      <c r="E56" s="351"/>
+      <c r="F56" s="351"/>
+      <c r="G56" s="351"/>
+      <c r="H56" s="351"/>
+      <c r="I56" s="351"/>
+      <c r="J56" s="351"/>
+      <c r="K56" s="351"/>
       <c r="L56" s="480"/>
       <c r="M56" s="305"/>
       <c r="N56" s="305"/>
@@ -22842,7 +23300,9 @@
     </row>
     <row r="58" spans="2:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="175"/>
-      <c r="C58" s="485"/>
+      <c r="C58" s="485" t="s">
+        <v>136</v>
+      </c>
       <c r="D58" s="486"/>
       <c r="E58" s="487"/>
       <c r="F58" s="487"/>
@@ -22932,11 +23392,10 @@
       <c r="B63" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="S15:S16"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:L3"/>
     <mergeCell ref="N2:O3"/>
@@ -22944,10 +23403,13 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.27559055118110237" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>